<commit_message>
upload raw data to figshare
</commit_message>
<xml_diff>
--- a/input_scripts/test_results.xlsx
+++ b/input_scripts/test_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenyang/Dropbox (Princeton)/EcoSLIM_CONUS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/C/EcoSLIM_test/EcoSLIM4_2/input_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52A5BE0-6699-8C40-9D87-B34BE1CEF170}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1E67B0-20BD-C04C-BDF4-EA56F9F96475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29560" yWindow="460" windowWidth="32740" windowHeight="21140" activeTab="1" xr2:uid="{7C13306F-2A42-DF49-85E6-122069AE8023}"/>
+    <workbookView xWindow="29560" yWindow="460" windowWidth="32740" windowHeight="21140" xr2:uid="{7C13306F-2A42-DF49-85E6-122069AE8023}"/>
   </bookViews>
   <sheets>
     <sheet name="LW_test" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="115">
   <si>
     <t>src0</t>
   </si>
@@ -636,6 +636,12 @@
   </si>
   <si>
     <t>Here are the test results of test6 for NCP (it is moved here since more columns are needed for 8 MPI ranks while the above tests only need 4 columns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For raw data and scripts generating Figures S4-S6 and 6, please refer to </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.6084/m9.figshare.19642689</t>
   </si>
 </sst>
 </file>
@@ -1669,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D0AE01-19A7-A849-A110-A07C28FF4467}">
-  <dimension ref="A1:AJ26"/>
+  <dimension ref="A1:AJ29"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="S43" sqref="S43"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -2910,6 +2916,16 @@
         <v>86</v>
       </c>
     </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B29" s="64" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2919,7 +2935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D514B5E1-D915-E945-A864-D5FFA6BD2E7B}">
   <dimension ref="A1:AI56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="90" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>

</xml_diff>